<commit_message>
Minor spreadsheet changes to match with chart
</commit_message>
<xml_diff>
--- a/Test Case - 4/TC4_Results_C.xlsx
+++ b/Test Case - 4/TC4_Results_C.xlsx
@@ -835,17 +835,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -895,7 +898,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -943,6 +946,56 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1222,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M70" sqref="M70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,21 +1286,21 @@
     <col min="8" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="5" t="s">
         <v>71</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -1262,7 +1315,7 @@
       <c r="L1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>76</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -1271,41 +1324,45 @@
       <c r="O1" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="2"/>
+      <c r="M2" s="5"/>
       <c r="N2" s="4" t="s">
         <v>77</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1342,11 +1399,11 @@
       <c r="L3" t="b">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1383,11 +1440,11 @@
       <c r="L4" t="b">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1424,11 +1481,11 @@
       <c r="L5" t="b">
         <v>1</v>
       </c>
-      <c r="P5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1465,11 +1522,11 @@
       <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1506,11 +1563,11 @@
       <c r="L7" t="b">
         <v>1</v>
       </c>
-      <c r="P7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1547,11 +1604,11 @@
       <c r="L8" t="b">
         <v>1</v>
       </c>
-      <c r="P8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1588,11 +1645,11 @@
       <c r="L9" t="b">
         <v>1</v>
       </c>
-      <c r="P9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1629,11 +1686,11 @@
       <c r="L10" t="b">
         <v>1</v>
       </c>
-      <c r="P10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1670,11 +1727,11 @@
       <c r="L11" t="b">
         <v>1</v>
       </c>
-      <c r="P11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1711,11 +1768,11 @@
       <c r="L12" t="b">
         <v>1</v>
       </c>
-      <c r="P12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1752,11 +1809,11 @@
       <c r="L13" t="b">
         <v>1</v>
       </c>
-      <c r="P13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1793,11 +1850,11 @@
       <c r="L14" t="b">
         <v>1</v>
       </c>
-      <c r="P14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1834,11 +1891,11 @@
       <c r="L15" t="b">
         <v>1</v>
       </c>
-      <c r="P15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1875,11 +1932,11 @@
       <c r="L16" t="b">
         <v>1</v>
       </c>
-      <c r="P16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1916,11 +1973,11 @@
       <c r="L17" t="b">
         <v>1</v>
       </c>
-      <c r="P17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1957,11 +2014,11 @@
       <c r="L18" t="b">
         <v>1</v>
       </c>
-      <c r="P18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1998,11 +2055,11 @@
       <c r="L19" t="b">
         <v>1</v>
       </c>
-      <c r="P19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2039,11 +2096,11 @@
       <c r="L20" t="b">
         <v>1</v>
       </c>
-      <c r="P20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2080,11 +2137,11 @@
       <c r="L21" t="b">
         <v>1</v>
       </c>
-      <c r="P21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2121,11 +2178,11 @@
       <c r="L22" t="b">
         <v>1</v>
       </c>
-      <c r="P22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2162,11 +2219,11 @@
       <c r="L23" t="b">
         <v>1</v>
       </c>
-      <c r="P23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2203,11 +2260,11 @@
       <c r="L24" t="b">
         <v>1</v>
       </c>
-      <c r="P24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2244,11 +2301,11 @@
       <c r="L25" t="b">
         <v>1</v>
       </c>
-      <c r="P25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2285,11 +2342,11 @@
       <c r="L26" t="b">
         <v>1</v>
       </c>
-      <c r="P26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2326,11 +2383,11 @@
       <c r="L27" t="b">
         <v>1</v>
       </c>
-      <c r="P27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2367,11 +2424,11 @@
       <c r="L28" t="b">
         <v>1</v>
       </c>
-      <c r="P28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2408,11 +2465,11 @@
       <c r="L29" t="b">
         <v>1</v>
       </c>
-      <c r="P29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2449,11 +2506,11 @@
       <c r="L30" t="b">
         <v>1</v>
       </c>
-      <c r="P30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -2490,11 +2547,14 @@
       <c r="L31" t="b">
         <v>0</v>
       </c>
-      <c r="P31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" t="b">
+        <v>1</v>
+      </c>
+      <c r="R31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -2531,11 +2591,14 @@
       <c r="L32" t="b">
         <v>0</v>
       </c>
-      <c r="P32" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" t="b">
+        <v>1</v>
+      </c>
+      <c r="R32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>34</v>
       </c>
@@ -2572,11 +2635,11 @@
       <c r="L33" t="b">
         <v>1</v>
       </c>
-      <c r="P33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>35</v>
       </c>
@@ -2613,11 +2676,11 @@
       <c r="L34" t="b">
         <v>1</v>
       </c>
-      <c r="P34" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>36</v>
       </c>
@@ -2654,11 +2717,11 @@
       <c r="L35" t="b">
         <v>1</v>
       </c>
-      <c r="P35" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>37</v>
       </c>
@@ -2695,11 +2758,11 @@
       <c r="L36" t="b">
         <v>1</v>
       </c>
-      <c r="P36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>38</v>
       </c>
@@ -2736,11 +2799,11 @@
       <c r="L37" t="b">
         <v>1</v>
       </c>
-      <c r="P37" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>39</v>
       </c>
@@ -2777,11 +2840,11 @@
       <c r="L38" t="b">
         <v>1</v>
       </c>
-      <c r="P38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>40</v>
       </c>
@@ -2818,11 +2881,11 @@
       <c r="L39" t="b">
         <v>1</v>
       </c>
-      <c r="P39" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>41</v>
       </c>
@@ -2859,11 +2922,11 @@
       <c r="L40" t="b">
         <v>1</v>
       </c>
-      <c r="P40" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>42</v>
       </c>
@@ -2900,11 +2963,11 @@
       <c r="L41" t="b">
         <v>1</v>
       </c>
-      <c r="P41" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>43</v>
       </c>
@@ -2941,11 +3004,11 @@
       <c r="L42" t="b">
         <v>1</v>
       </c>
-      <c r="P42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>49</v>
       </c>
@@ -2982,11 +3045,11 @@
       <c r="L43" t="b">
         <v>1</v>
       </c>
-      <c r="P43" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>57</v>
       </c>
@@ -3023,11 +3086,11 @@
       <c r="L44" t="b">
         <v>1</v>
       </c>
-      <c r="P44" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>58</v>
       </c>
@@ -3064,11 +3127,11 @@
       <c r="L45" t="b">
         <v>1</v>
       </c>
-      <c r="P45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>59</v>
       </c>
@@ -3105,11 +3168,11 @@
       <c r="L46" t="b">
         <v>1</v>
       </c>
-      <c r="P46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60</v>
       </c>
@@ -3146,11 +3209,11 @@
       <c r="L47" t="b">
         <v>1</v>
       </c>
-      <c r="P47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>61</v>
       </c>
@@ -3187,11 +3250,11 @@
       <c r="L48" t="b">
         <v>1</v>
       </c>
-      <c r="P48" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>62</v>
       </c>
@@ -3228,11 +3291,11 @@
       <c r="L49" t="b">
         <v>1</v>
       </c>
-      <c r="P49" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>64</v>
       </c>
@@ -3269,11 +3332,11 @@
       <c r="L50" t="b">
         <v>1</v>
       </c>
-      <c r="P50" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>65</v>
       </c>
@@ -3310,11 +3373,11 @@
       <c r="L51" t="b">
         <v>1</v>
       </c>
-      <c r="P51" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>66</v>
       </c>
@@ -3351,11 +3414,11 @@
       <c r="L52" t="b">
         <v>1</v>
       </c>
-      <c r="P52" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>67</v>
       </c>
@@ -3392,11 +3455,11 @@
       <c r="L53" t="b">
         <v>1</v>
       </c>
-      <c r="P53" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>68</v>
       </c>
@@ -3433,11 +3496,11 @@
       <c r="L54" t="b">
         <v>1</v>
       </c>
-      <c r="P54" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>69</v>
       </c>
@@ -3474,11 +3537,11 @@
       <c r="L55" t="b">
         <v>1</v>
       </c>
-      <c r="P55" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>70</v>
       </c>
@@ -3515,11 +3578,11 @@
       <c r="L56" t="b">
         <v>1</v>
       </c>
-      <c r="P56" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>71</v>
       </c>
@@ -3556,11 +3619,11 @@
       <c r="L57" t="b">
         <v>1</v>
       </c>
-      <c r="P57" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>72</v>
       </c>
@@ -3597,11 +3660,11 @@
       <c r="L58" t="b">
         <v>1</v>
       </c>
-      <c r="P58" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>73</v>
       </c>
@@ -3638,11 +3701,11 @@
       <c r="L59" t="b">
         <v>1</v>
       </c>
-      <c r="P59" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>74</v>
       </c>
@@ -3684,11 +3747,15 @@
       </c>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
-      <c r="P60" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P60" s="2"/>
+      <c r="Q60" t="b">
+        <v>1</v>
+      </c>
+      <c r="R60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>76</v>
       </c>
@@ -3728,11 +3795,15 @@
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
-      <c r="P61" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P61" s="2"/>
+      <c r="Q61" t="b">
+        <v>1</v>
+      </c>
+      <c r="R61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>77</v>
       </c>
@@ -3772,11 +3843,15 @@
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
-      <c r="P62" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P62" s="2"/>
+      <c r="Q62" t="b">
+        <v>1</v>
+      </c>
+      <c r="R62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>78</v>
       </c>
@@ -3816,11 +3891,15 @@
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
-      <c r="P63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P63" s="2"/>
+      <c r="Q63" t="b">
+        <v>1</v>
+      </c>
+      <c r="R63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>80</v>
       </c>
@@ -3860,11 +3939,15 @@
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
-      <c r="P64" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P64" s="2"/>
+      <c r="Q64" t="b">
+        <v>1</v>
+      </c>
+      <c r="R64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>81</v>
       </c>
@@ -3904,11 +3987,15 @@
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
-      <c r="P65" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P65" s="2"/>
+      <c r="Q65" t="b">
+        <v>1</v>
+      </c>
+      <c r="R65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>82</v>
       </c>
@@ -3948,11 +4035,15 @@
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
-      <c r="P66" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P66" s="2"/>
+      <c r="Q66" t="b">
+        <v>1</v>
+      </c>
+      <c r="R66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>83</v>
       </c>
@@ -3989,11 +4080,15 @@
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
-      <c r="P67" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P67" s="2"/>
+      <c r="Q67" t="b">
+        <v>1</v>
+      </c>
+      <c r="R67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>85</v>
       </c>
@@ -4030,11 +4125,15 @@
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
-      <c r="P68" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P68" s="2"/>
+      <c r="Q68" t="b">
+        <v>1</v>
+      </c>
+      <c r="R68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>86</v>
       </c>
@@ -4071,12 +4170,20 @@
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
-      <c r="P69" t="s">
+      <c r="P69" s="2"/>
+      <c r="Q69" t="b">
+        <v>1</v>
+      </c>
+      <c r="R69" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M60:O69"/>
@@ -4085,12 +4192,32 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L30 L33:L69">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L31:L32">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q60:Q69">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q31">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4098,7 +4225,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L31:L32">
+  <conditionalFormatting sqref="Q32">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>